<commit_message>
improve value saving logic
</commit_message>
<xml_diff>
--- a/Projects/Mars Thallo/model_value_tracking/output/sorted_ot_data_20240827_20240828.xlsx
+++ b/Projects/Mars Thallo/model_value_tracking/output/sorted_ot_data_20240827_20240828.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E339"/>
+  <dimension ref="A1:E346"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2532,16 +2532,18 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_Gap3rdSizing.rActualPosition_inches</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_Gap2ndSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C111" s="2" t="n">
-        <v>45531.875</v>
+        <v>45532.32304398148</v>
       </c>
       <c r="D111" t="n">
-        <v>0.0737</v>
-      </c>
-      <c r="E111" t="inlineStr"/>
+        <v>0.0762</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.0764</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -2553,14 +2555,12 @@
         </is>
       </c>
       <c r="C112" s="2" t="n">
-        <v>45531.8779050926</v>
+        <v>45531.875</v>
       </c>
       <c r="D112" t="n">
-        <v>0.0722</v>
-      </c>
-      <c r="E112" t="n">
         <v>0.0737</v>
       </c>
+      <c r="E112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -2572,13 +2572,13 @@
         </is>
       </c>
       <c r="C113" s="2" t="n">
-        <v>45531.87791666666</v>
+        <v>45531.8779050926</v>
       </c>
       <c r="D113" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.0722</v>
       </c>
       <c r="E113" t="n">
-        <v>0.0722</v>
+        <v>0.0737</v>
       </c>
     </row>
     <row r="114">
@@ -2591,13 +2591,13 @@
         </is>
       </c>
       <c r="C114" s="2" t="n">
-        <v>45531.89015046296</v>
+        <v>45531.87791666666</v>
       </c>
       <c r="D114" t="n">
-        <v>0.08550000000000001</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="E114" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.0722</v>
       </c>
     </row>
     <row r="115">
@@ -2610,13 +2610,13 @@
         </is>
       </c>
       <c r="C115" s="2" t="n">
-        <v>45531.89016203704</v>
+        <v>45531.89015046296</v>
       </c>
       <c r="D115" t="n">
-        <v>0.0988</v>
+        <v>0.08550000000000001</v>
       </c>
       <c r="E115" t="n">
-        <v>0.08550000000000001</v>
+        <v>0.07140000000000001</v>
       </c>
     </row>
     <row r="116">
@@ -2629,13 +2629,13 @@
         </is>
       </c>
       <c r="C116" s="2" t="n">
-        <v>45531.89017361111</v>
+        <v>45531.89016203704</v>
       </c>
       <c r="D116" t="n">
-        <v>0.1221</v>
+        <v>0.0988</v>
       </c>
       <c r="E116" t="n">
-        <v>0.0988</v>
+        <v>0.08550000000000001</v>
       </c>
     </row>
     <row r="117">
@@ -2648,13 +2648,13 @@
         </is>
       </c>
       <c r="C117" s="2" t="n">
-        <v>45531.89018518518</v>
+        <v>45531.89017361111</v>
       </c>
       <c r="D117" t="n">
-        <v>0.1439</v>
+        <v>0.1221</v>
       </c>
       <c r="E117" t="n">
-        <v>0.1221</v>
+        <v>0.0988</v>
       </c>
     </row>
     <row r="118">
@@ -2667,13 +2667,13 @@
         </is>
       </c>
       <c r="C118" s="2" t="n">
-        <v>45531.89027777778</v>
+        <v>45531.89018518518</v>
       </c>
       <c r="D118" t="n">
-        <v>0.1312</v>
+        <v>0.1439</v>
       </c>
       <c r="E118" t="n">
-        <v>0.1439</v>
+        <v>0.1221</v>
       </c>
     </row>
     <row r="119">
@@ -2686,13 +2686,13 @@
         </is>
       </c>
       <c r="C119" s="2" t="n">
-        <v>45531.89028935185</v>
+        <v>45531.89027777778</v>
       </c>
       <c r="D119" t="n">
-        <v>0.1023</v>
+        <v>0.1312</v>
       </c>
       <c r="E119" t="n">
-        <v>0.1312</v>
+        <v>0.1439</v>
       </c>
     </row>
     <row r="120">
@@ -2705,13 +2705,13 @@
         </is>
       </c>
       <c r="C120" s="2" t="n">
-        <v>45531.89099537037</v>
+        <v>45531.89028935185</v>
       </c>
       <c r="D120" t="n">
-        <v>0.0857</v>
+        <v>0.1023</v>
       </c>
       <c r="E120" t="n">
-        <v>0.1023</v>
+        <v>0.1312</v>
       </c>
     </row>
     <row r="121">
@@ -2724,13 +2724,13 @@
         </is>
       </c>
       <c r="C121" s="2" t="n">
-        <v>45531.89100694445</v>
+        <v>45531.89099537037</v>
       </c>
       <c r="D121" t="n">
-        <v>0.0751</v>
+        <v>0.0857</v>
       </c>
       <c r="E121" t="n">
-        <v>0.0857</v>
+        <v>0.1023</v>
       </c>
     </row>
     <row r="122">
@@ -2743,13 +2743,13 @@
         </is>
       </c>
       <c r="C122" s="2" t="n">
-        <v>45531.89101851852</v>
+        <v>45531.89100694445</v>
       </c>
       <c r="D122" t="n">
-        <v>0.0701</v>
+        <v>0.0751</v>
       </c>
       <c r="E122" t="n">
-        <v>0.0751</v>
+        <v>0.0857</v>
       </c>
     </row>
     <row r="123">
@@ -2762,13 +2762,13 @@
         </is>
       </c>
       <c r="C123" s="2" t="n">
-        <v>45531.89103009259</v>
+        <v>45531.89101851852</v>
       </c>
       <c r="D123" t="n">
-        <v>0.0716</v>
+        <v>0.0701</v>
       </c>
       <c r="E123" t="n">
-        <v>0.0701</v>
+        <v>0.0751</v>
       </c>
     </row>
     <row r="124">
@@ -2781,13 +2781,13 @@
         </is>
       </c>
       <c r="C124" s="2" t="n">
-        <v>45531.92153935185</v>
+        <v>45531.89103009259</v>
       </c>
       <c r="D124" t="n">
-        <v>0.0702</v>
+        <v>0.0716</v>
       </c>
       <c r="E124" t="n">
-        <v>0.0716</v>
+        <v>0.0701</v>
       </c>
     </row>
     <row r="125">
@@ -2800,13 +2800,13 @@
         </is>
       </c>
       <c r="C125" s="2" t="n">
-        <v>45531.92322916666</v>
+        <v>45531.92152777778</v>
       </c>
       <c r="D125" t="n">
-        <v>0.0692</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="E125" t="n">
-        <v>0.0702</v>
+        <v>0.0716</v>
       </c>
     </row>
     <row r="126">
@@ -2819,13 +2819,13 @@
         </is>
       </c>
       <c r="C126" s="2" t="n">
-        <v>45531.93805555555</v>
+        <v>45531.92153935185</v>
       </c>
       <c r="D126" t="n">
-        <v>0.082</v>
+        <v>0.0702</v>
       </c>
       <c r="E126" t="n">
-        <v>0.0692</v>
+        <v>0.07099999999999999</v>
       </c>
     </row>
     <row r="127">
@@ -2838,13 +2838,13 @@
         </is>
       </c>
       <c r="C127" s="2" t="n">
-        <v>45531.93806712963</v>
+        <v>45531.92322916666</v>
       </c>
       <c r="D127" t="n">
-        <v>0.09429999999999999</v>
+        <v>0.0692</v>
       </c>
       <c r="E127" t="n">
-        <v>0.082</v>
+        <v>0.0702</v>
       </c>
     </row>
     <row r="128">
@@ -2857,13 +2857,13 @@
         </is>
       </c>
       <c r="C128" s="2" t="n">
-        <v>45531.9380787037</v>
+        <v>45531.93805555555</v>
       </c>
       <c r="D128" t="n">
-        <v>0.1088</v>
+        <v>0.082</v>
       </c>
       <c r="E128" t="n">
-        <v>0.09429999999999999</v>
+        <v>0.0692</v>
       </c>
     </row>
     <row r="129">
@@ -2876,13 +2876,13 @@
         </is>
       </c>
       <c r="C129" s="2" t="n">
-        <v>45531.93809027778</v>
+        <v>45531.93806712963</v>
       </c>
       <c r="D129" t="n">
-        <v>0.1199</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="E129" t="n">
-        <v>0.1088</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="130">
@@ -2895,13 +2895,13 @@
         </is>
       </c>
       <c r="C130" s="2" t="n">
-        <v>45531.93900462963</v>
+        <v>45531.9380787037</v>
       </c>
       <c r="D130" t="n">
-        <v>0.1027</v>
+        <v>0.1088</v>
       </c>
       <c r="E130" t="n">
-        <v>0.1199</v>
+        <v>0.09429999999999999</v>
       </c>
     </row>
     <row r="131">
@@ -2914,13 +2914,13 @@
         </is>
       </c>
       <c r="C131" s="2" t="n">
-        <v>45531.9390162037</v>
+        <v>45531.93809027778</v>
       </c>
       <c r="D131" t="n">
-        <v>0.0878</v>
+        <v>0.1199</v>
       </c>
       <c r="E131" t="n">
-        <v>0.1027</v>
+        <v>0.1088</v>
       </c>
     </row>
     <row r="132">
@@ -2933,13 +2933,13 @@
         </is>
       </c>
       <c r="C132" s="2" t="n">
-        <v>45531.93902777778</v>
+        <v>45531.93900462963</v>
       </c>
       <c r="D132" t="n">
-        <v>0.0757</v>
+        <v>0.1027</v>
       </c>
       <c r="E132" t="n">
-        <v>0.0878</v>
+        <v>0.1199</v>
       </c>
     </row>
     <row r="133">
@@ -2952,13 +2952,13 @@
         </is>
       </c>
       <c r="C133" s="2" t="n">
-        <v>45531.93903935186</v>
+        <v>45531.9390162037</v>
       </c>
       <c r="D133" t="n">
-        <v>0.0732</v>
+        <v>0.0878</v>
       </c>
       <c r="E133" t="n">
-        <v>0.0757</v>
+        <v>0.1027</v>
       </c>
     </row>
     <row r="134">
@@ -2971,13 +2971,13 @@
         </is>
       </c>
       <c r="C134" s="2" t="n">
-        <v>45531.94332175926</v>
+        <v>45531.93902777778</v>
       </c>
       <c r="D134" t="n">
-        <v>0.0717</v>
+        <v>0.0757</v>
       </c>
       <c r="E134" t="n">
-        <v>0.0732</v>
+        <v>0.0878</v>
       </c>
     </row>
     <row r="135">
@@ -2990,13 +2990,13 @@
         </is>
       </c>
       <c r="C135" s="2" t="n">
-        <v>45531.94333333334</v>
+        <v>45531.93903935186</v>
       </c>
       <c r="D135" t="n">
-        <v>0.0702</v>
+        <v>0.0732</v>
       </c>
       <c r="E135" t="n">
-        <v>0.0717</v>
+        <v>0.0757</v>
       </c>
     </row>
     <row r="136">
@@ -3009,13 +3009,13 @@
         </is>
       </c>
       <c r="C136" s="2" t="n">
-        <v>45531.97688657408</v>
+        <v>45531.94332175926</v>
       </c>
       <c r="D136" t="n">
-        <v>0.1074</v>
+        <v>0.0717</v>
       </c>
       <c r="E136" t="n">
-        <v>0.0702</v>
+        <v>0.0732</v>
       </c>
     </row>
     <row r="137">
@@ -3028,13 +3028,13 @@
         </is>
       </c>
       <c r="C137" s="2" t="n">
-        <v>45531.97689814815</v>
+        <v>45531.94333333334</v>
       </c>
       <c r="D137" t="n">
-        <v>0.1213</v>
+        <v>0.0702</v>
       </c>
       <c r="E137" t="n">
-        <v>0.1074</v>
+        <v>0.0717</v>
       </c>
     </row>
     <row r="138">
@@ -3047,13 +3047,13 @@
         </is>
       </c>
       <c r="C138" s="2" t="n">
-        <v>45531.97690972222</v>
+        <v>45531.97688657408</v>
       </c>
       <c r="D138" t="n">
-        <v>0.1455</v>
+        <v>0.1074</v>
       </c>
       <c r="E138" t="n">
-        <v>0.1213</v>
+        <v>0.0702</v>
       </c>
     </row>
     <row r="139">
@@ -3066,13 +3066,13 @@
         </is>
       </c>
       <c r="C139" s="2" t="n">
-        <v>45531.97692129629</v>
+        <v>45531.97689814815</v>
       </c>
       <c r="D139" t="n">
-        <v>0.1572</v>
+        <v>0.1213</v>
       </c>
       <c r="E139" t="n">
-        <v>0.1455</v>
+        <v>0.1074</v>
       </c>
     </row>
     <row r="140">
@@ -3085,13 +3085,13 @@
         </is>
       </c>
       <c r="C140" s="2" t="n">
-        <v>45531.97697916667</v>
+        <v>45531.97690972222</v>
       </c>
       <c r="D140" t="n">
-        <v>0.1459</v>
+        <v>0.1455</v>
       </c>
       <c r="E140" t="n">
-        <v>0.1572</v>
+        <v>0.1213</v>
       </c>
     </row>
     <row r="141">
@@ -3104,13 +3104,13 @@
         </is>
       </c>
       <c r="C141" s="2" t="n">
-        <v>45531.97699074074</v>
+        <v>45531.97692129629</v>
       </c>
       <c r="D141" t="n">
-        <v>0.1198</v>
+        <v>0.1572</v>
       </c>
       <c r="E141" t="n">
-        <v>0.1459</v>
+        <v>0.1455</v>
       </c>
     </row>
     <row r="142">
@@ -3123,13 +3123,13 @@
         </is>
       </c>
       <c r="C142" s="2" t="n">
-        <v>45531.97700231482</v>
+        <v>45531.97697916667</v>
       </c>
       <c r="D142" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.1459</v>
       </c>
       <c r="E142" t="n">
-        <v>0.1198</v>
+        <v>0.1572</v>
       </c>
     </row>
     <row r="143">
@@ -3142,13 +3142,13 @@
         </is>
       </c>
       <c r="C143" s="2" t="n">
-        <v>45531.97701388889</v>
+        <v>45531.97699074074</v>
       </c>
       <c r="D143" t="n">
-        <v>0.0747</v>
+        <v>0.1198</v>
       </c>
       <c r="E143" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.1459</v>
       </c>
     </row>
     <row r="144">
@@ -3161,13 +3161,13 @@
         </is>
       </c>
       <c r="C144" s="2" t="n">
-        <v>45531.97702546296</v>
+        <v>45531.97700231482</v>
       </c>
       <c r="D144" t="n">
-        <v>0.0718</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="E144" t="n">
-        <v>0.0747</v>
+        <v>0.1198</v>
       </c>
     </row>
     <row r="145">
@@ -3180,13 +3180,13 @@
         </is>
       </c>
       <c r="C145" s="2" t="n">
-        <v>45531.98252314814</v>
+        <v>45531.97701388889</v>
       </c>
       <c r="D145" t="n">
-        <v>0.0696</v>
+        <v>0.0747</v>
       </c>
       <c r="E145" t="n">
-        <v>0.0718</v>
+        <v>0.08500000000000001</v>
       </c>
     </row>
     <row r="146">
@@ -3199,13 +3199,13 @@
         </is>
       </c>
       <c r="C146" s="2" t="n">
-        <v>45532.0549537037</v>
+        <v>45531.97702546296</v>
       </c>
       <c r="D146" t="n">
-        <v>0.0829</v>
+        <v>0.0718</v>
       </c>
       <c r="E146" t="n">
-        <v>0.0696</v>
+        <v>0.0747</v>
       </c>
     </row>
     <row r="147">
@@ -3218,13 +3218,13 @@
         </is>
       </c>
       <c r="C147" s="2" t="n">
-        <v>45532.05496527778</v>
+        <v>45531.98251157408</v>
       </c>
       <c r="D147" t="n">
-        <v>0.1055</v>
+        <v>0.0711</v>
       </c>
       <c r="E147" t="n">
-        <v>0.0829</v>
+        <v>0.0718</v>
       </c>
     </row>
     <row r="148">
@@ -3237,13 +3237,13 @@
         </is>
       </c>
       <c r="C148" s="2" t="n">
-        <v>45532.05497685185</v>
+        <v>45531.98252314814</v>
       </c>
       <c r="D148" t="n">
-        <v>0.1356</v>
+        <v>0.0696</v>
       </c>
       <c r="E148" t="n">
-        <v>0.1055</v>
+        <v>0.0711</v>
       </c>
     </row>
     <row r="149">
@@ -3256,13 +3256,13 @@
         </is>
       </c>
       <c r="C149" s="2" t="n">
-        <v>45532.05498842592</v>
+        <v>45532.0549537037</v>
       </c>
       <c r="D149" t="n">
-        <v>0.1674</v>
+        <v>0.0829</v>
       </c>
       <c r="E149" t="n">
-        <v>0.1356</v>
+        <v>0.0696</v>
       </c>
     </row>
     <row r="150">
@@ -3275,13 +3275,13 @@
         </is>
       </c>
       <c r="C150" s="2" t="n">
-        <v>45532.055</v>
+        <v>45532.05496527778</v>
       </c>
       <c r="D150" t="n">
-        <v>0.184</v>
+        <v>0.1055</v>
       </c>
       <c r="E150" t="n">
-        <v>0.1674</v>
+        <v>0.0829</v>
       </c>
     </row>
     <row r="151">
@@ -3294,13 +3294,13 @@
         </is>
       </c>
       <c r="C151" s="2" t="n">
-        <v>45532.05521990741</v>
+        <v>45532.05497685185</v>
       </c>
       <c r="D151" t="n">
-        <v>0.1738</v>
+        <v>0.1356</v>
       </c>
       <c r="E151" t="n">
-        <v>0.184</v>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="152">
@@ -3313,13 +3313,13 @@
         </is>
       </c>
       <c r="C152" s="2" t="n">
-        <v>45532.05523148148</v>
+        <v>45532.05498842592</v>
       </c>
       <c r="D152" t="n">
-        <v>0.1509</v>
+        <v>0.1674</v>
       </c>
       <c r="E152" t="n">
-        <v>0.1738</v>
+        <v>0.1356</v>
       </c>
     </row>
     <row r="153">
@@ -3332,13 +3332,13 @@
         </is>
       </c>
       <c r="C153" s="2" t="n">
-        <v>45532.05524305555</v>
+        <v>45532.055</v>
       </c>
       <c r="D153" t="n">
-        <v>0.1299</v>
+        <v>0.184</v>
       </c>
       <c r="E153" t="n">
-        <v>0.1509</v>
+        <v>0.1674</v>
       </c>
     </row>
     <row r="154">
@@ -3351,13 +3351,13 @@
         </is>
       </c>
       <c r="C154" s="2" t="n">
-        <v>45532.05525462963</v>
+        <v>45532.05521990741</v>
       </c>
       <c r="D154" t="n">
-        <v>0.1079</v>
+        <v>0.1738</v>
       </c>
       <c r="E154" t="n">
-        <v>0.1299</v>
+        <v>0.184</v>
       </c>
     </row>
     <row r="155">
@@ -3370,13 +3370,13 @@
         </is>
       </c>
       <c r="C155" s="2" t="n">
-        <v>45532.0552662037</v>
+        <v>45532.05523148148</v>
       </c>
       <c r="D155" t="n">
-        <v>0.0915</v>
+        <v>0.1509</v>
       </c>
       <c r="E155" t="n">
-        <v>0.1079</v>
+        <v>0.1738</v>
       </c>
     </row>
     <row r="156">
@@ -3389,13 +3389,13 @@
         </is>
       </c>
       <c r="C156" s="2" t="n">
-        <v>45532.05527777778</v>
+        <v>45532.05524305555</v>
       </c>
       <c r="D156" t="n">
-        <v>0.0838</v>
+        <v>0.1299</v>
       </c>
       <c r="E156" t="n">
-        <v>0.0915</v>
+        <v>0.1509</v>
       </c>
     </row>
     <row r="157">
@@ -3408,13 +3408,13 @@
         </is>
       </c>
       <c r="C157" s="2" t="n">
-        <v>45532.05528935185</v>
+        <v>45532.05525462963</v>
       </c>
       <c r="D157" t="n">
-        <v>0.07630000000000001</v>
+        <v>0.1079</v>
       </c>
       <c r="E157" t="n">
-        <v>0.0838</v>
+        <v>0.1299</v>
       </c>
     </row>
     <row r="158">
@@ -3427,13 +3427,13 @@
         </is>
       </c>
       <c r="C158" s="2" t="n">
-        <v>45532.05530092592</v>
+        <v>45532.0552662037</v>
       </c>
       <c r="D158" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.0915</v>
       </c>
       <c r="E158" t="n">
-        <v>0.07630000000000001</v>
+        <v>0.1079</v>
       </c>
     </row>
     <row r="159">
@@ -3446,13 +3446,13 @@
         </is>
       </c>
       <c r="C159" s="2" t="n">
-        <v>45532.05982638889</v>
+        <v>45532.05527777778</v>
       </c>
       <c r="D159" t="n">
-        <v>0.07049999999999999</v>
+        <v>0.0838</v>
       </c>
       <c r="E159" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.0915</v>
       </c>
     </row>
     <row r="160">
@@ -3465,13 +3465,13 @@
         </is>
       </c>
       <c r="C160" s="2" t="n">
-        <v>45532.09288194445</v>
+        <v>45532.05528935185</v>
       </c>
       <c r="D160" t="n">
-        <v>0.0717</v>
+        <v>0.07630000000000001</v>
       </c>
       <c r="E160" t="n">
-        <v>0.07049999999999999</v>
+        <v>0.0838</v>
       </c>
     </row>
     <row r="161">
@@ -3484,13 +3484,13 @@
         </is>
       </c>
       <c r="C161" s="2" t="n">
-        <v>45532.09289351852</v>
+        <v>45532.05530092592</v>
       </c>
       <c r="D161" t="n">
-        <v>0.09429999999999999</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="E161" t="n">
-        <v>0.0717</v>
+        <v>0.07630000000000001</v>
       </c>
     </row>
     <row r="162">
@@ -3503,13 +3503,13 @@
         </is>
       </c>
       <c r="C162" s="2" t="n">
-        <v>45532.09290509259</v>
+        <v>45532.05538194445</v>
       </c>
       <c r="D162" t="n">
-        <v>0.1168</v>
+        <v>0.0721</v>
       </c>
       <c r="E162" t="n">
-        <v>0.09429999999999999</v>
+        <v>0.07140000000000001</v>
       </c>
     </row>
     <row r="163">
@@ -3522,13 +3522,13 @@
         </is>
       </c>
       <c r="C163" s="2" t="n">
-        <v>45532.09291666667</v>
+        <v>45532.05982638889</v>
       </c>
       <c r="D163" t="n">
-        <v>0.1335</v>
+        <v>0.07049999999999999</v>
       </c>
       <c r="E163" t="n">
-        <v>0.1168</v>
+        <v>0.0721</v>
       </c>
     </row>
     <row r="164">
@@ -3541,13 +3541,13 @@
         </is>
       </c>
       <c r="C164" s="2" t="n">
-        <v>45532.09292824074</v>
+        <v>45532.09288194445</v>
       </c>
       <c r="D164" t="n">
-        <v>0.1405</v>
+        <v>0.0717</v>
       </c>
       <c r="E164" t="n">
-        <v>0.1335</v>
+        <v>0.07049999999999999</v>
       </c>
     </row>
     <row r="165">
@@ -3560,13 +3560,13 @@
         </is>
       </c>
       <c r="C165" s="2" t="n">
-        <v>45532.09300925926</v>
+        <v>45532.09289351852</v>
       </c>
       <c r="D165" t="n">
-        <v>0.1223</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="E165" t="n">
-        <v>0.1405</v>
+        <v>0.0717</v>
       </c>
     </row>
     <row r="166">
@@ -3579,13 +3579,13 @@
         </is>
       </c>
       <c r="C166" s="2" t="n">
-        <v>45532.09302083333</v>
+        <v>45532.09290509259</v>
       </c>
       <c r="D166" t="n">
-        <v>0.0925</v>
+        <v>0.1168</v>
       </c>
       <c r="E166" t="n">
-        <v>0.1223</v>
+        <v>0.09429999999999999</v>
       </c>
     </row>
     <row r="167">
@@ -3598,13 +3598,13 @@
         </is>
       </c>
       <c r="C167" s="2" t="n">
-        <v>45532.09303240741</v>
+        <v>45532.09291666667</v>
       </c>
       <c r="D167" t="n">
-        <v>0.0658</v>
+        <v>0.1335</v>
       </c>
       <c r="E167" t="n">
-        <v>0.0925</v>
+        <v>0.1168</v>
       </c>
     </row>
     <row r="168">
@@ -3617,13 +3617,13 @@
         </is>
       </c>
       <c r="C168" s="2" t="n">
-        <v>45532.09304398148</v>
+        <v>45532.09292824074</v>
       </c>
       <c r="D168" t="n">
-        <v>0.0694</v>
+        <v>0.1405</v>
       </c>
       <c r="E168" t="n">
-        <v>0.0658</v>
+        <v>0.1335</v>
       </c>
     </row>
     <row r="169">
@@ -3636,13 +3636,13 @@
         </is>
       </c>
       <c r="C169" s="2" t="n">
-        <v>45532.09305555555</v>
+        <v>45532.09300925926</v>
       </c>
       <c r="D169" t="n">
-        <v>0.0701</v>
+        <v>0.1223</v>
       </c>
       <c r="E169" t="n">
-        <v>0.0694</v>
+        <v>0.1405</v>
       </c>
     </row>
     <row r="170">
@@ -3655,13 +3655,13 @@
         </is>
       </c>
       <c r="C170" s="2" t="n">
-        <v>45532.09567129629</v>
+        <v>45532.09302083333</v>
       </c>
       <c r="D170" t="n">
-        <v>0.07290000000000001</v>
+        <v>0.0925</v>
       </c>
       <c r="E170" t="n">
-        <v>0.0701</v>
+        <v>0.1223</v>
       </c>
     </row>
     <row r="171">
@@ -3674,13 +3674,13 @@
         </is>
       </c>
       <c r="C171" s="2" t="n">
-        <v>45532.09730324074</v>
+        <v>45532.09303240741</v>
       </c>
       <c r="D171" t="n">
-        <v>0.0721</v>
+        <v>0.0658</v>
       </c>
       <c r="E171" t="n">
-        <v>0.07290000000000001</v>
+        <v>0.0925</v>
       </c>
     </row>
     <row r="172">
@@ -3693,13 +3693,13 @@
         </is>
       </c>
       <c r="C172" s="2" t="n">
-        <v>45532.09731481481</v>
+        <v>45532.09304398148</v>
       </c>
       <c r="D172" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.0694</v>
       </c>
       <c r="E172" t="n">
-        <v>0.0721</v>
+        <v>0.0658</v>
       </c>
     </row>
     <row r="173">
@@ -3712,13 +3712,13 @@
         </is>
       </c>
       <c r="C173" s="2" t="n">
-        <v>45532.13283564815</v>
+        <v>45532.09305555555</v>
       </c>
       <c r="D173" t="n">
-        <v>0.0732</v>
+        <v>0.0701</v>
       </c>
       <c r="E173" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.0694</v>
       </c>
     </row>
     <row r="174">
@@ -3731,13 +3731,13 @@
         </is>
       </c>
       <c r="C174" s="2" t="n">
-        <v>45532.13400462963</v>
+        <v>45532.09567129629</v>
       </c>
       <c r="D174" t="n">
-        <v>0.07190000000000001</v>
+        <v>0.07290000000000001</v>
       </c>
       <c r="E174" t="n">
-        <v>0.0732</v>
+        <v>0.0701</v>
       </c>
     </row>
     <row r="175">
@@ -3750,13 +3750,13 @@
         </is>
       </c>
       <c r="C175" s="2" t="n">
-        <v>45532.1340162037</v>
+        <v>45532.09730324074</v>
       </c>
       <c r="D175" t="n">
-        <v>0.0706</v>
+        <v>0.0721</v>
       </c>
       <c r="E175" t="n">
-        <v>0.07190000000000001</v>
+        <v>0.07290000000000001</v>
       </c>
     </row>
     <row r="176">
@@ -3769,13 +3769,13 @@
         </is>
       </c>
       <c r="C176" s="2" t="n">
-        <v>45532.19857638889</v>
+        <v>45532.09731481481</v>
       </c>
       <c r="D176" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="E176" t="n">
-        <v>0.0706</v>
+        <v>0.0721</v>
       </c>
     </row>
     <row r="177">
@@ -3788,13 +3788,13 @@
         </is>
       </c>
       <c r="C177" s="2" t="n">
-        <v>45532.22407407407</v>
+        <v>45532.1328125</v>
       </c>
       <c r="D177" t="n">
-        <v>0.0701</v>
+        <v>0.0706</v>
       </c>
       <c r="E177" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.07099999999999999</v>
       </c>
     </row>
     <row r="178">
@@ -3807,13 +3807,13 @@
         </is>
       </c>
       <c r="C178" s="2" t="n">
-        <v>45532.2241087963</v>
+        <v>45532.13283564815</v>
       </c>
       <c r="D178" t="n">
-        <v>0.0693</v>
+        <v>0.0732</v>
       </c>
       <c r="E178" t="n">
-        <v>0.0701</v>
+        <v>0.0706</v>
       </c>
     </row>
     <row r="179">
@@ -3826,13 +3826,13 @@
         </is>
       </c>
       <c r="C179" s="2" t="n">
-        <v>45532.24736111111</v>
+        <v>45532.13400462963</v>
       </c>
       <c r="D179" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.07190000000000001</v>
       </c>
       <c r="E179" t="n">
-        <v>0.0693</v>
+        <v>0.0732</v>
       </c>
     </row>
     <row r="180">
@@ -3845,13 +3845,13 @@
         </is>
       </c>
       <c r="C180" s="2" t="n">
-        <v>45532.25435185185</v>
+        <v>45532.1340162037</v>
       </c>
       <c r="D180" t="n">
-        <v>0.06909999999999999</v>
+        <v>0.0706</v>
       </c>
       <c r="E180" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.07190000000000001</v>
       </c>
     </row>
     <row r="181">
@@ -3864,13 +3864,13 @@
         </is>
       </c>
       <c r="C181" s="2" t="n">
-        <v>45532.27678240741</v>
+        <v>45532.19856481482</v>
       </c>
       <c r="D181" t="n">
-        <v>0.0709</v>
+        <v>0.0707</v>
       </c>
       <c r="E181" t="n">
-        <v>0.06909999999999999</v>
+        <v>0.0706</v>
       </c>
     </row>
     <row r="182">
@@ -3883,13 +3883,13 @@
         </is>
       </c>
       <c r="C182" s="2" t="n">
-        <v>45532.27680555556</v>
+        <v>45532.19857638889</v>
       </c>
       <c r="D182" t="n">
         <v>0.07199999999999999</v>
       </c>
       <c r="E182" t="n">
-        <v>0.0709</v>
+        <v>0.0707</v>
       </c>
     </row>
     <row r="183">
@@ -3902,10 +3902,10 @@
         </is>
       </c>
       <c r="C183" s="2" t="n">
-        <v>45532.28555555556</v>
+        <v>45532.22407407407</v>
       </c>
       <c r="D183" t="n">
-        <v>0.0704</v>
+        <v>0.0701</v>
       </c>
       <c r="E183" t="n">
         <v>0.07199999999999999</v>
@@ -3921,13 +3921,13 @@
         </is>
       </c>
       <c r="C184" s="2" t="n">
-        <v>45532.28556712963</v>
+        <v>45532.2241087963</v>
       </c>
       <c r="D184" t="n">
-        <v>0.0696</v>
+        <v>0.0693</v>
       </c>
       <c r="E184" t="n">
-        <v>0.0704</v>
+        <v>0.0701</v>
       </c>
     </row>
     <row r="185">
@@ -3940,13 +3940,13 @@
         </is>
       </c>
       <c r="C185" s="2" t="n">
-        <v>45532.30432870371</v>
+        <v>45532.22465277778</v>
       </c>
       <c r="D185" t="n">
-        <v>0.0716</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="E185" t="n">
-        <v>0.0696</v>
+        <v>0.0693</v>
       </c>
     </row>
     <row r="186">
@@ -3959,13 +3959,13 @@
         </is>
       </c>
       <c r="C186" s="2" t="n">
-        <v>45532.31008101852</v>
+        <v>45532.24736111111</v>
       </c>
       <c r="D186" t="n">
-        <v>0.0704</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E186" t="n">
-        <v>0.0716</v>
+        <v>0.06900000000000001</v>
       </c>
     </row>
     <row r="187">
@@ -3978,13 +3978,13 @@
         </is>
       </c>
       <c r="C187" s="2" t="n">
-        <v>45532.31009259259</v>
+        <v>45532.25435185185</v>
       </c>
       <c r="D187" t="n">
-        <v>0.0696</v>
+        <v>0.06909999999999999</v>
       </c>
       <c r="E187" t="n">
-        <v>0.0704</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="188">
@@ -3997,13 +3997,13 @@
         </is>
       </c>
       <c r="C188" s="2" t="n">
-        <v>45532.323125</v>
+        <v>45532.27678240741</v>
       </c>
       <c r="D188" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.0709</v>
       </c>
       <c r="E188" t="n">
-        <v>0.0696</v>
+        <v>0.06909999999999999</v>
       </c>
     </row>
     <row r="189">
@@ -4016,13 +4016,13 @@
         </is>
       </c>
       <c r="C189" s="2" t="n">
-        <v>45532.32314814815</v>
+        <v>45532.27680555556</v>
       </c>
       <c r="D189" t="n">
-        <v>0.0723</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="E189" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.0709</v>
       </c>
     </row>
     <row r="190">
@@ -4035,13 +4035,13 @@
         </is>
       </c>
       <c r="C190" s="2" t="n">
-        <v>45532.32998842592</v>
+        <v>45532.28555555556</v>
       </c>
       <c r="D190" t="n">
-        <v>0.07149999999999999</v>
+        <v>0.0704</v>
       </c>
       <c r="E190" t="n">
-        <v>0.0723</v>
+        <v>0.07199999999999999</v>
       </c>
     </row>
     <row r="191">
@@ -4054,13 +4054,13 @@
         </is>
       </c>
       <c r="C191" s="2" t="n">
-        <v>45532.33001157407</v>
+        <v>45532.28556712963</v>
       </c>
       <c r="D191" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.0696</v>
       </c>
       <c r="E191" t="n">
-        <v>0.07149999999999999</v>
+        <v>0.0704</v>
       </c>
     </row>
     <row r="192">
@@ -4069,16 +4069,18 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_Gap3rdSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C192" s="2" t="n">
-        <v>45531.875</v>
+        <v>45532.30432870371</v>
       </c>
       <c r="D192" t="n">
-        <v>0.0648</v>
-      </c>
-      <c r="E192" t="inlineStr"/>
+        <v>0.0716</v>
+      </c>
+      <c r="E192" t="n">
+        <v>0.0696</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -4086,17 +4088,17 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_Gap3rdSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C193" s="2" t="n">
-        <v>45531.89021990741</v>
+        <v>45532.31008101852</v>
       </c>
       <c r="D193" t="n">
-        <v>0.0796</v>
+        <v>0.0704</v>
       </c>
       <c r="E193" t="n">
-        <v>0.0648</v>
+        <v>0.0716</v>
       </c>
     </row>
     <row r="194">
@@ -4105,17 +4107,17 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_Gap3rdSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C194" s="2" t="n">
-        <v>45531.89024305555</v>
+        <v>45532.31009259259</v>
       </c>
       <c r="D194" t="n">
-        <v>0.1083</v>
+        <v>0.0696</v>
       </c>
       <c r="E194" t="n">
-        <v>0.0796</v>
+        <v>0.0704</v>
       </c>
     </row>
     <row r="195">
@@ -4124,17 +4126,17 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_Gap3rdSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C195" s="2" t="n">
-        <v>45531.89024305555</v>
+        <v>45532.323125</v>
       </c>
       <c r="D195" t="n">
-        <v>0.1211</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="E195" t="n">
-        <v>0.1083</v>
+        <v>0.0696</v>
       </c>
     </row>
     <row r="196">
@@ -4143,17 +4145,17 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_Gap3rdSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C196" s="2" t="n">
-        <v>45531.89025462963</v>
+        <v>45532.32314814815</v>
       </c>
       <c r="D196" t="n">
-        <v>0.1436</v>
+        <v>0.0723</v>
       </c>
       <c r="E196" t="n">
-        <v>0.1211</v>
+        <v>0.07099999999999999</v>
       </c>
     </row>
     <row r="197">
@@ -4162,17 +4164,17 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_Gap3rdSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C197" s="2" t="n">
-        <v>45531.89026620371</v>
+        <v>45532.32998842592</v>
       </c>
       <c r="D197" t="n">
-        <v>0.1535</v>
+        <v>0.07149999999999999</v>
       </c>
       <c r="E197" t="n">
-        <v>0.1436</v>
+        <v>0.0723</v>
       </c>
     </row>
     <row r="198">
@@ -4181,17 +4183,17 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_Gap3rdSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C198" s="2" t="n">
-        <v>45531.89027777778</v>
+        <v>45532.33001157407</v>
       </c>
       <c r="D198" t="n">
-        <v>0.1591</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E198" t="n">
-        <v>0.1535</v>
+        <v>0.07149999999999999</v>
       </c>
     </row>
     <row r="199">
@@ -4204,14 +4206,12 @@
         </is>
       </c>
       <c r="C199" s="2" t="n">
-        <v>45531.89028935185</v>
+        <v>45531.875</v>
       </c>
       <c r="D199" t="n">
-        <v>0.1609</v>
-      </c>
-      <c r="E199" t="n">
-        <v>0.1591</v>
-      </c>
+        <v>0.0648</v>
+      </c>
+      <c r="E199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -4223,13 +4223,13 @@
         </is>
       </c>
       <c r="C200" s="2" t="n">
-        <v>45531.8903125</v>
+        <v>45531.89021990741</v>
       </c>
       <c r="D200" t="n">
-        <v>0.1647</v>
+        <v>0.0796</v>
       </c>
       <c r="E200" t="n">
-        <v>0.1609</v>
+        <v>0.0648</v>
       </c>
     </row>
     <row r="201">
@@ -4242,13 +4242,13 @@
         </is>
       </c>
       <c r="C201" s="2" t="n">
-        <v>45531.89063657408</v>
+        <v>45531.89024305555</v>
       </c>
       <c r="D201" t="n">
-        <v>0.1754</v>
+        <v>0.1083</v>
       </c>
       <c r="E201" t="n">
-        <v>0.1647</v>
+        <v>0.0796</v>
       </c>
     </row>
     <row r="202">
@@ -4261,13 +4261,13 @@
         </is>
       </c>
       <c r="C202" s="2" t="n">
-        <v>45531.89064814815</v>
+        <v>45531.89024305555</v>
       </c>
       <c r="D202" t="n">
-        <v>0.1901</v>
+        <v>0.1211</v>
       </c>
       <c r="E202" t="n">
-        <v>0.1754</v>
+        <v>0.1083</v>
       </c>
     </row>
     <row r="203">
@@ -4280,13 +4280,13 @@
         </is>
       </c>
       <c r="C203" s="2" t="n">
-        <v>45531.89065972222</v>
+        <v>45531.89025462963</v>
       </c>
       <c r="D203" t="n">
-        <v>0.2012</v>
+        <v>0.1436</v>
       </c>
       <c r="E203" t="n">
-        <v>0.1901</v>
+        <v>0.1211</v>
       </c>
     </row>
     <row r="204">
@@ -4299,13 +4299,13 @@
         </is>
       </c>
       <c r="C204" s="2" t="n">
-        <v>45531.8906712963</v>
+        <v>45531.89026620371</v>
       </c>
       <c r="D204" t="n">
-        <v>0.2047</v>
+        <v>0.1535</v>
       </c>
       <c r="E204" t="n">
-        <v>0.2012</v>
+        <v>0.1436</v>
       </c>
     </row>
     <row r="205">
@@ -4318,13 +4318,13 @@
         </is>
       </c>
       <c r="C205" s="2" t="n">
-        <v>45531.89105324074</v>
+        <v>45531.89027777778</v>
       </c>
       <c r="D205" t="n">
-        <v>0.22</v>
+        <v>0.1591</v>
       </c>
       <c r="E205" t="n">
-        <v>0.2047</v>
+        <v>0.1535</v>
       </c>
     </row>
     <row r="206">
@@ -4337,13 +4337,13 @@
         </is>
       </c>
       <c r="C206" s="2" t="n">
-        <v>45531.89105324074</v>
+        <v>45531.89028935185</v>
       </c>
       <c r="D206" t="n">
-        <v>0.2352</v>
+        <v>0.1609</v>
       </c>
       <c r="E206" t="n">
-        <v>0.22</v>
+        <v>0.1591</v>
       </c>
     </row>
     <row r="207">
@@ -4356,13 +4356,13 @@
         </is>
       </c>
       <c r="C207" s="2" t="n">
-        <v>45531.8950462963</v>
+        <v>45531.8903125</v>
       </c>
       <c r="D207" t="n">
-        <v>0.2052</v>
+        <v>0.1647</v>
       </c>
       <c r="E207" t="n">
-        <v>0.2352</v>
+        <v>0.1609</v>
       </c>
     </row>
     <row r="208">
@@ -4375,13 +4375,13 @@
         </is>
       </c>
       <c r="C208" s="2" t="n">
-        <v>45531.89506944444</v>
+        <v>45531.89063657408</v>
       </c>
       <c r="D208" t="n">
-        <v>0.1898</v>
+        <v>0.1754</v>
       </c>
       <c r="E208" t="n">
-        <v>0.2052</v>
+        <v>0.1647</v>
       </c>
     </row>
     <row r="209">
@@ -4394,13 +4394,13 @@
         </is>
       </c>
       <c r="C209" s="2" t="n">
-        <v>45531.89509259259</v>
+        <v>45531.89064814815</v>
       </c>
       <c r="D209" t="n">
-        <v>0.1585</v>
+        <v>0.1901</v>
       </c>
       <c r="E209" t="n">
-        <v>0.1898</v>
+        <v>0.1754</v>
       </c>
     </row>
     <row r="210">
@@ -4413,13 +4413,13 @@
         </is>
       </c>
       <c r="C210" s="2" t="n">
-        <v>45531.89510416667</v>
+        <v>45531.89065972222</v>
       </c>
       <c r="D210" t="n">
-        <v>0.1425</v>
+        <v>0.2012</v>
       </c>
       <c r="E210" t="n">
-        <v>0.1585</v>
+        <v>0.1901</v>
       </c>
     </row>
     <row r="211">
@@ -4432,13 +4432,13 @@
         </is>
       </c>
       <c r="C211" s="2" t="n">
-        <v>45531.89511574074</v>
+        <v>45531.8906712963</v>
       </c>
       <c r="D211" t="n">
-        <v>0.1111</v>
+        <v>0.2047</v>
       </c>
       <c r="E211" t="n">
-        <v>0.1425</v>
+        <v>0.2012</v>
       </c>
     </row>
     <row r="212">
@@ -4451,13 +4451,13 @@
         </is>
       </c>
       <c r="C212" s="2" t="n">
-        <v>45531.89511574074</v>
+        <v>45531.89105324074</v>
       </c>
       <c r="D212" t="n">
-        <v>0.096</v>
+        <v>0.22</v>
       </c>
       <c r="E212" t="n">
-        <v>0.1111</v>
+        <v>0.2047</v>
       </c>
     </row>
     <row r="213">
@@ -4470,13 +4470,13 @@
         </is>
       </c>
       <c r="C213" s="2" t="n">
-        <v>45531.89512731481</v>
+        <v>45531.89105324074</v>
       </c>
       <c r="D213" t="n">
-        <v>0.08019999999999999</v>
+        <v>0.2352</v>
       </c>
       <c r="E213" t="n">
-        <v>0.096</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="214">
@@ -4489,13 +4489,13 @@
         </is>
       </c>
       <c r="C214" s="2" t="n">
-        <v>45531.89513888889</v>
+        <v>45531.8950462963</v>
       </c>
       <c r="D214" t="n">
-        <v>0.0639</v>
+        <v>0.2052</v>
       </c>
       <c r="E214" t="n">
-        <v>0.08019999999999999</v>
+        <v>0.2352</v>
       </c>
     </row>
     <row r="215">
@@ -4508,13 +4508,13 @@
         </is>
       </c>
       <c r="C215" s="2" t="n">
-        <v>45531.89516203704</v>
+        <v>45531.89506944444</v>
       </c>
       <c r="D215" t="n">
-        <v>0.065</v>
+        <v>0.1898</v>
       </c>
       <c r="E215" t="n">
-        <v>0.0639</v>
+        <v>0.2052</v>
       </c>
     </row>
     <row r="216">
@@ -4527,13 +4527,13 @@
         </is>
       </c>
       <c r="C216" s="2" t="n">
-        <v>45531.92163194445</v>
+        <v>45531.89509259259</v>
       </c>
       <c r="D216" t="n">
-        <v>0.06419999999999999</v>
+        <v>0.1585</v>
       </c>
       <c r="E216" t="n">
-        <v>0.065</v>
+        <v>0.1898</v>
       </c>
     </row>
     <row r="217">
@@ -4546,13 +4546,13 @@
         </is>
       </c>
       <c r="C217" s="2" t="n">
-        <v>45531.92165509259</v>
+        <v>45531.89510416667</v>
       </c>
       <c r="D217" t="n">
-        <v>0.063</v>
+        <v>0.1425</v>
       </c>
       <c r="E217" t="n">
-        <v>0.06419999999999999</v>
+        <v>0.1585</v>
       </c>
     </row>
     <row r="218">
@@ -4565,13 +4565,13 @@
         </is>
       </c>
       <c r="C218" s="2" t="n">
-        <v>45531.93819444445</v>
+        <v>45531.89511574074</v>
       </c>
       <c r="D218" t="n">
-        <v>0.0696</v>
+        <v>0.1111</v>
       </c>
       <c r="E218" t="n">
-        <v>0.063</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="219">
@@ -4584,13 +4584,13 @@
         </is>
       </c>
       <c r="C219" s="2" t="n">
-        <v>45531.93820601852</v>
+        <v>45531.89511574074</v>
       </c>
       <c r="D219" t="n">
-        <v>0.0786</v>
+        <v>0.096</v>
       </c>
       <c r="E219" t="n">
-        <v>0.0696</v>
+        <v>0.1111</v>
       </c>
     </row>
     <row r="220">
@@ -4603,13 +4603,13 @@
         </is>
       </c>
       <c r="C220" s="2" t="n">
-        <v>45531.93821759259</v>
+        <v>45531.89512731481</v>
       </c>
       <c r="D220" t="n">
-        <v>0.0795</v>
+        <v>0.08019999999999999</v>
       </c>
       <c r="E220" t="n">
-        <v>0.0786</v>
+        <v>0.096</v>
       </c>
     </row>
     <row r="221">
@@ -4622,13 +4622,13 @@
         </is>
       </c>
       <c r="C221" s="2" t="n">
-        <v>45531.93822916667</v>
+        <v>45531.89513888889</v>
       </c>
       <c r="D221" t="n">
-        <v>0.0833</v>
+        <v>0.0639</v>
       </c>
       <c r="E221" t="n">
-        <v>0.0795</v>
+        <v>0.08019999999999999</v>
       </c>
     </row>
     <row r="222">
@@ -4641,13 +4641,13 @@
         </is>
       </c>
       <c r="C222" s="2" t="n">
-        <v>45531.93824074074</v>
+        <v>45531.89516203704</v>
       </c>
       <c r="D222" t="n">
-        <v>0.08459999999999999</v>
+        <v>0.065</v>
       </c>
       <c r="E222" t="n">
-        <v>0.0833</v>
+        <v>0.0639</v>
       </c>
     </row>
     <row r="223">
@@ -4660,13 +4660,13 @@
         </is>
       </c>
       <c r="C223" s="2" t="n">
-        <v>45531.93826388889</v>
+        <v>45531.92163194445</v>
       </c>
       <c r="D223" t="n">
-        <v>0.0863</v>
+        <v>0.06419999999999999</v>
       </c>
       <c r="E223" t="n">
-        <v>0.08459999999999999</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="224">
@@ -4679,13 +4679,13 @@
         </is>
       </c>
       <c r="C224" s="2" t="n">
-        <v>45531.93940972222</v>
+        <v>45531.92165509259</v>
       </c>
       <c r="D224" t="n">
-        <v>0.1009</v>
+        <v>0.063</v>
       </c>
       <c r="E224" t="n">
-        <v>0.0863</v>
+        <v>0.06419999999999999</v>
       </c>
     </row>
     <row r="225">
@@ -4698,13 +4698,13 @@
         </is>
       </c>
       <c r="C225" s="2" t="n">
-        <v>45531.93942129629</v>
+        <v>45531.93819444445</v>
       </c>
       <c r="D225" t="n">
-        <v>0.1285</v>
+        <v>0.0696</v>
       </c>
       <c r="E225" t="n">
-        <v>0.1009</v>
+        <v>0.063</v>
       </c>
     </row>
     <row r="226">
@@ -4717,13 +4717,13 @@
         </is>
       </c>
       <c r="C226" s="2" t="n">
-        <v>45531.93943287037</v>
+        <v>45531.93820601852</v>
       </c>
       <c r="D226" t="n">
-        <v>0.1495</v>
+        <v>0.0786</v>
       </c>
       <c r="E226" t="n">
-        <v>0.1285</v>
+        <v>0.0696</v>
       </c>
     </row>
     <row r="227">
@@ -4736,13 +4736,13 @@
         </is>
       </c>
       <c r="C227" s="2" t="n">
-        <v>45531.93944444445</v>
+        <v>45531.93821759259</v>
       </c>
       <c r="D227" t="n">
-        <v>0.1631</v>
+        <v>0.0795</v>
       </c>
       <c r="E227" t="n">
-        <v>0.1495</v>
+        <v>0.0786</v>
       </c>
     </row>
     <row r="228">
@@ -4755,13 +4755,13 @@
         </is>
       </c>
       <c r="C228" s="2" t="n">
-        <v>45531.93947916666</v>
+        <v>45531.93822916667</v>
       </c>
       <c r="D228" t="n">
-        <v>0.19</v>
+        <v>0.0833</v>
       </c>
       <c r="E228" t="n">
-        <v>0.1631</v>
+        <v>0.0795</v>
       </c>
     </row>
     <row r="229">
@@ -4774,13 +4774,13 @@
         </is>
       </c>
       <c r="C229" s="2" t="n">
-        <v>45531.93949074074</v>
+        <v>45531.93824074074</v>
       </c>
       <c r="D229" t="n">
-        <v>0.2002</v>
+        <v>0.08459999999999999</v>
       </c>
       <c r="E229" t="n">
-        <v>0.19</v>
+        <v>0.0833</v>
       </c>
     </row>
     <row r="230">
@@ -4793,13 +4793,13 @@
         </is>
       </c>
       <c r="C230" s="2" t="n">
-        <v>45531.93953703704</v>
+        <v>45531.93826388889</v>
       </c>
       <c r="D230" t="n">
-        <v>0.2077</v>
+        <v>0.0863</v>
       </c>
       <c r="E230" t="n">
-        <v>0.2002</v>
+        <v>0.08459999999999999</v>
       </c>
     </row>
     <row r="231">
@@ -4812,13 +4812,13 @@
         </is>
       </c>
       <c r="C231" s="2" t="n">
-        <v>45531.94119212963</v>
+        <v>45531.93940972222</v>
       </c>
       <c r="D231" t="n">
-        <v>0.193</v>
+        <v>0.1009</v>
       </c>
       <c r="E231" t="n">
-        <v>0.2077</v>
+        <v>0.0863</v>
       </c>
     </row>
     <row r="232">
@@ -4831,13 +4831,13 @@
         </is>
       </c>
       <c r="C232" s="2" t="n">
-        <v>45531.9412037037</v>
+        <v>45531.93942129629</v>
       </c>
       <c r="D232" t="n">
-        <v>0.1655</v>
+        <v>0.1285</v>
       </c>
       <c r="E232" t="n">
-        <v>0.193</v>
+        <v>0.1009</v>
       </c>
     </row>
     <row r="233">
@@ -4850,13 +4850,13 @@
         </is>
       </c>
       <c r="C233" s="2" t="n">
-        <v>45531.94122685185</v>
+        <v>45531.93943287037</v>
       </c>
       <c r="D233" t="n">
-        <v>0.1492</v>
+        <v>0.1495</v>
       </c>
       <c r="E233" t="n">
-        <v>0.1655</v>
+        <v>0.1285</v>
       </c>
     </row>
     <row r="234">
@@ -4869,13 +4869,13 @@
         </is>
       </c>
       <c r="C234" s="2" t="n">
-        <v>45531.94123842593</v>
+        <v>45531.93944444445</v>
       </c>
       <c r="D234" t="n">
-        <v>0.1171</v>
+        <v>0.1631</v>
       </c>
       <c r="E234" t="n">
-        <v>0.1492</v>
+        <v>0.1495</v>
       </c>
     </row>
     <row r="235">
@@ -4888,13 +4888,13 @@
         </is>
       </c>
       <c r="C235" s="2" t="n">
-        <v>45531.94125</v>
+        <v>45531.93947916666</v>
       </c>
       <c r="D235" t="n">
-        <v>0.1053</v>
+        <v>0.19</v>
       </c>
       <c r="E235" t="n">
-        <v>0.1171</v>
+        <v>0.1631</v>
       </c>
     </row>
     <row r="236">
@@ -4907,13 +4907,13 @@
         </is>
       </c>
       <c r="C236" s="2" t="n">
-        <v>45531.94126157407</v>
+        <v>45531.93949074074</v>
       </c>
       <c r="D236" t="n">
-        <v>0.09039999999999999</v>
+        <v>0.2002</v>
       </c>
       <c r="E236" t="n">
-        <v>0.1053</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="237">
@@ -4926,13 +4926,13 @@
         </is>
       </c>
       <c r="C237" s="2" t="n">
-        <v>45531.94127314815</v>
+        <v>45531.93953703704</v>
       </c>
       <c r="D237" t="n">
-        <v>0.0679</v>
+        <v>0.2077</v>
       </c>
       <c r="E237" t="n">
-        <v>0.09039999999999999</v>
+        <v>0.2002</v>
       </c>
     </row>
     <row r="238">
@@ -4945,13 +4945,13 @@
         </is>
       </c>
       <c r="C238" s="2" t="n">
-        <v>45531.94128472222</v>
+        <v>45531.94119212963</v>
       </c>
       <c r="D238" t="n">
-        <v>0.0643</v>
+        <v>0.193</v>
       </c>
       <c r="E238" t="n">
-        <v>0.0679</v>
+        <v>0.2077</v>
       </c>
     </row>
     <row r="239">
@@ -4964,13 +4964,13 @@
         </is>
       </c>
       <c r="C239" s="2" t="n">
-        <v>45531.9412962963</v>
+        <v>45531.9412037037</v>
       </c>
       <c r="D239" t="n">
-        <v>0.0633</v>
+        <v>0.1655</v>
       </c>
       <c r="E239" t="n">
-        <v>0.0643</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="240">
@@ -4983,13 +4983,13 @@
         </is>
       </c>
       <c r="C240" s="2" t="n">
-        <v>45531.97766203704</v>
+        <v>45531.94122685185</v>
       </c>
       <c r="D240" t="n">
-        <v>0.08019999999999999</v>
+        <v>0.1492</v>
       </c>
       <c r="E240" t="n">
-        <v>0.0633</v>
+        <v>0.1655</v>
       </c>
     </row>
     <row r="241">
@@ -5002,13 +5002,13 @@
         </is>
       </c>
       <c r="C241" s="2" t="n">
-        <v>45531.97767361111</v>
+        <v>45531.94123842593</v>
       </c>
       <c r="D241" t="n">
-        <v>0.0949</v>
+        <v>0.1171</v>
       </c>
       <c r="E241" t="n">
-        <v>0.08019999999999999</v>
+        <v>0.1492</v>
       </c>
     </row>
     <row r="242">
@@ -5021,13 +5021,13 @@
         </is>
       </c>
       <c r="C242" s="2" t="n">
-        <v>45531.97768518519</v>
+        <v>45531.94125</v>
       </c>
       <c r="D242" t="n">
-        <v>0.1214</v>
+        <v>0.1053</v>
       </c>
       <c r="E242" t="n">
-        <v>0.0949</v>
+        <v>0.1171</v>
       </c>
     </row>
     <row r="243">
@@ -5040,13 +5040,13 @@
         </is>
       </c>
       <c r="C243" s="2" t="n">
-        <v>45531.97769675926</v>
+        <v>45531.94126157407</v>
       </c>
       <c r="D243" t="n">
-        <v>0.133</v>
+        <v>0.09039999999999999</v>
       </c>
       <c r="E243" t="n">
-        <v>0.1214</v>
+        <v>0.1053</v>
       </c>
     </row>
     <row r="244">
@@ -5059,13 +5059,13 @@
         </is>
       </c>
       <c r="C244" s="2" t="n">
-        <v>45531.97815972222</v>
+        <v>45531.94127314815</v>
       </c>
       <c r="D244" t="n">
-        <v>0.1474</v>
+        <v>0.0679</v>
       </c>
       <c r="E244" t="n">
-        <v>0.133</v>
+        <v>0.09039999999999999</v>
       </c>
     </row>
     <row r="245">
@@ -5078,13 +5078,13 @@
         </is>
       </c>
       <c r="C245" s="2" t="n">
-        <v>45531.97817129629</v>
+        <v>45531.94128472222</v>
       </c>
       <c r="D245" t="n">
-        <v>0.1739</v>
+        <v>0.0643</v>
       </c>
       <c r="E245" t="n">
-        <v>0.1474</v>
+        <v>0.0679</v>
       </c>
     </row>
     <row r="246">
@@ -5097,13 +5097,13 @@
         </is>
       </c>
       <c r="C246" s="2" t="n">
-        <v>45531.97818287037</v>
+        <v>45531.9412962963</v>
       </c>
       <c r="D246" t="n">
-        <v>0.1856</v>
+        <v>0.0633</v>
       </c>
       <c r="E246" t="n">
-        <v>0.1739</v>
+        <v>0.0643</v>
       </c>
     </row>
     <row r="247">
@@ -5116,13 +5116,13 @@
         </is>
       </c>
       <c r="C247" s="2" t="n">
-        <v>45531.97833333333</v>
+        <v>45531.97766203704</v>
       </c>
       <c r="D247" t="n">
-        <v>0.2002</v>
+        <v>0.08019999999999999</v>
       </c>
       <c r="E247" t="n">
-        <v>0.1856</v>
+        <v>0.0633</v>
       </c>
     </row>
     <row r="248">
@@ -5135,13 +5135,13 @@
         </is>
       </c>
       <c r="C248" s="2" t="n">
-        <v>45531.97834490741</v>
+        <v>45531.97767361111</v>
       </c>
       <c r="D248" t="n">
-        <v>0.2126</v>
+        <v>0.0949</v>
       </c>
       <c r="E248" t="n">
-        <v>0.2002</v>
+        <v>0.08019999999999999</v>
       </c>
     </row>
     <row r="249">
@@ -5154,13 +5154,13 @@
         </is>
       </c>
       <c r="C249" s="2" t="n">
-        <v>45531.97959490741</v>
+        <v>45531.97768518519</v>
       </c>
       <c r="D249" t="n">
-        <v>0.1815</v>
+        <v>0.1214</v>
       </c>
       <c r="E249" t="n">
-        <v>0.2126</v>
+        <v>0.0949</v>
       </c>
     </row>
     <row r="250">
@@ -5173,13 +5173,13 @@
         </is>
       </c>
       <c r="C250" s="2" t="n">
-        <v>45531.97960648148</v>
+        <v>45531.97769675926</v>
       </c>
       <c r="D250" t="n">
-        <v>0.1456</v>
+        <v>0.133</v>
       </c>
       <c r="E250" t="n">
-        <v>0.1815</v>
+        <v>0.1214</v>
       </c>
     </row>
     <row r="251">
@@ -5192,13 +5192,13 @@
         </is>
       </c>
       <c r="C251" s="2" t="n">
-        <v>45531.97961805556</v>
+        <v>45531.97815972222</v>
       </c>
       <c r="D251" t="n">
-        <v>0.129</v>
+        <v>0.1474</v>
       </c>
       <c r="E251" t="n">
-        <v>0.1456</v>
+        <v>0.133</v>
       </c>
     </row>
     <row r="252">
@@ -5211,13 +5211,13 @@
         </is>
       </c>
       <c r="C252" s="2" t="n">
-        <v>45531.97962962963</v>
+        <v>45531.97817129629</v>
       </c>
       <c r="D252" t="n">
-        <v>0.1108</v>
+        <v>0.1739</v>
       </c>
       <c r="E252" t="n">
-        <v>0.129</v>
+        <v>0.1474</v>
       </c>
     </row>
     <row r="253">
@@ -5230,13 +5230,13 @@
         </is>
       </c>
       <c r="C253" s="2" t="n">
-        <v>45531.9796412037</v>
+        <v>45531.97818287037</v>
       </c>
       <c r="D253" t="n">
-        <v>0.0921</v>
+        <v>0.1856</v>
       </c>
       <c r="E253" t="n">
-        <v>0.1108</v>
+        <v>0.1739</v>
       </c>
     </row>
     <row r="254">
@@ -5249,13 +5249,13 @@
         </is>
       </c>
       <c r="C254" s="2" t="n">
-        <v>45531.97966435185</v>
+        <v>45531.97833333333</v>
       </c>
       <c r="D254" t="n">
-        <v>0.0629</v>
+        <v>0.2002</v>
       </c>
       <c r="E254" t="n">
-        <v>0.0921</v>
+        <v>0.1856</v>
       </c>
     </row>
     <row r="255">
@@ -5268,13 +5268,13 @@
         </is>
       </c>
       <c r="C255" s="2" t="n">
-        <v>45531.97967592593</v>
+        <v>45531.97834490741</v>
       </c>
       <c r="D255" t="n">
-        <v>0.06419999999999999</v>
+        <v>0.2126</v>
       </c>
       <c r="E255" t="n">
-        <v>0.0629</v>
+        <v>0.2002</v>
       </c>
     </row>
     <row r="256">
@@ -5287,13 +5287,13 @@
         </is>
       </c>
       <c r="C256" s="2" t="n">
-        <v>45532.02615740741</v>
+        <v>45531.97959490741</v>
       </c>
       <c r="D256" t="n">
-        <v>0.078</v>
+        <v>0.1815</v>
       </c>
       <c r="E256" t="n">
-        <v>0.06419999999999999</v>
+        <v>0.2126</v>
       </c>
     </row>
     <row r="257">
@@ -5306,13 +5306,13 @@
         </is>
       </c>
       <c r="C257" s="2" t="n">
-        <v>45532.02616898148</v>
+        <v>45531.97960648148</v>
       </c>
       <c r="D257" t="n">
-        <v>0.1073</v>
+        <v>0.1456</v>
       </c>
       <c r="E257" t="n">
-        <v>0.078</v>
+        <v>0.1815</v>
       </c>
     </row>
     <row r="258">
@@ -5325,13 +5325,13 @@
         </is>
       </c>
       <c r="C258" s="2" t="n">
-        <v>45532.02618055556</v>
+        <v>45531.97961805556</v>
       </c>
       <c r="D258" t="n">
-        <v>0.1237</v>
+        <v>0.129</v>
       </c>
       <c r="E258" t="n">
-        <v>0.1073</v>
+        <v>0.1456</v>
       </c>
     </row>
     <row r="259">
@@ -5344,13 +5344,13 @@
         </is>
       </c>
       <c r="C259" s="2" t="n">
-        <v>45532.02619212963</v>
+        <v>45531.97962962963</v>
       </c>
       <c r="D259" t="n">
-        <v>0.1483</v>
+        <v>0.1108</v>
       </c>
       <c r="E259" t="n">
-        <v>0.1237</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="260">
@@ -5363,13 +5363,13 @@
         </is>
       </c>
       <c r="C260" s="2" t="n">
-        <v>45532.0262037037</v>
+        <v>45531.9796412037</v>
       </c>
       <c r="D260" t="n">
-        <v>0.1695</v>
+        <v>0.0921</v>
       </c>
       <c r="E260" t="n">
-        <v>0.1483</v>
+        <v>0.1108</v>
       </c>
     </row>
     <row r="261">
@@ -5382,13 +5382,13 @@
         </is>
       </c>
       <c r="C261" s="2" t="n">
-        <v>45532.02621527778</v>
+        <v>45531.97966435185</v>
       </c>
       <c r="D261" t="n">
-        <v>0.1844</v>
+        <v>0.0629</v>
       </c>
       <c r="E261" t="n">
-        <v>0.1695</v>
+        <v>0.0921</v>
       </c>
     </row>
     <row r="262">
@@ -5401,13 +5401,13 @@
         </is>
       </c>
       <c r="C262" s="2" t="n">
-        <v>45532.02622685185</v>
+        <v>45531.97967592593</v>
       </c>
       <c r="D262" t="n">
-        <v>0.1868</v>
+        <v>0.06419999999999999</v>
       </c>
       <c r="E262" t="n">
-        <v>0.1844</v>
+        <v>0.0629</v>
       </c>
     </row>
     <row r="263">
@@ -5420,13 +5420,13 @@
         </is>
       </c>
       <c r="C263" s="2" t="n">
-        <v>45532.02623842593</v>
+        <v>45532.02615740741</v>
       </c>
       <c r="D263" t="n">
-        <v>0.1906</v>
+        <v>0.078</v>
       </c>
       <c r="E263" t="n">
-        <v>0.1868</v>
+        <v>0.06419999999999999</v>
       </c>
     </row>
     <row r="264">
@@ -5439,13 +5439,13 @@
         </is>
       </c>
       <c r="C264" s="2" t="n">
-        <v>45532.04225694444</v>
+        <v>45532.02616898148</v>
       </c>
       <c r="D264" t="n">
-        <v>0.1618</v>
+        <v>0.1073</v>
       </c>
       <c r="E264" t="n">
-        <v>0.1906</v>
+        <v>0.078</v>
       </c>
     </row>
     <row r="265">
@@ -5458,13 +5458,13 @@
         </is>
       </c>
       <c r="C265" s="2" t="n">
-        <v>45532.04226851852</v>
+        <v>45532.02618055556</v>
       </c>
       <c r="D265" t="n">
-        <v>0.1375</v>
+        <v>0.1237</v>
       </c>
       <c r="E265" t="n">
-        <v>0.1618</v>
+        <v>0.1073</v>
       </c>
     </row>
     <row r="266">
@@ -5477,13 +5477,13 @@
         </is>
       </c>
       <c r="C266" s="2" t="n">
-        <v>45532.0422800926</v>
+        <v>45532.02619212963</v>
       </c>
       <c r="D266" t="n">
-        <v>0.114</v>
+        <v>0.1483</v>
       </c>
       <c r="E266" t="n">
-        <v>0.1375</v>
+        <v>0.1237</v>
       </c>
     </row>
     <row r="267">
@@ -5496,13 +5496,13 @@
         </is>
       </c>
       <c r="C267" s="2" t="n">
-        <v>45532.04229166666</v>
+        <v>45532.0262037037</v>
       </c>
       <c r="D267" t="n">
-        <v>0.0924</v>
+        <v>0.1695</v>
       </c>
       <c r="E267" t="n">
-        <v>0.114</v>
+        <v>0.1483</v>
       </c>
     </row>
     <row r="268">
@@ -5515,13 +5515,13 @@
         </is>
       </c>
       <c r="C268" s="2" t="n">
-        <v>45532.04230324074</v>
+        <v>45532.02621527778</v>
       </c>
       <c r="D268" t="n">
-        <v>0.0716</v>
+        <v>0.1844</v>
       </c>
       <c r="E268" t="n">
-        <v>0.0924</v>
+        <v>0.1695</v>
       </c>
     </row>
     <row r="269">
@@ -5534,13 +5534,13 @@
         </is>
       </c>
       <c r="C269" s="2" t="n">
-        <v>45532.04236111111</v>
+        <v>45532.02622685185</v>
       </c>
       <c r="D269" t="n">
-        <v>0.0602</v>
+        <v>0.1868</v>
       </c>
       <c r="E269" t="n">
-        <v>0.0716</v>
+        <v>0.1844</v>
       </c>
     </row>
     <row r="270">
@@ -5553,13 +5553,13 @@
         </is>
       </c>
       <c r="C270" s="2" t="n">
-        <v>45532.04238425926</v>
+        <v>45532.02623842593</v>
       </c>
       <c r="D270" t="n">
-        <v>0.06419999999999999</v>
+        <v>0.1906</v>
       </c>
       <c r="E270" t="n">
-        <v>0.0602</v>
+        <v>0.1868</v>
       </c>
     </row>
     <row r="271">
@@ -5572,13 +5572,13 @@
         </is>
       </c>
       <c r="C271" s="2" t="n">
-        <v>45532.09120370371</v>
+        <v>45532.04225694444</v>
       </c>
       <c r="D271" t="n">
-        <v>0.0718</v>
+        <v>0.1618</v>
       </c>
       <c r="E271" t="n">
-        <v>0.06419999999999999</v>
+        <v>0.1906</v>
       </c>
     </row>
     <row r="272">
@@ -5591,13 +5591,13 @@
         </is>
       </c>
       <c r="C272" s="2" t="n">
-        <v>45532.09121527777</v>
+        <v>45532.04226851852</v>
       </c>
       <c r="D272" t="n">
-        <v>0.1088</v>
+        <v>0.1375</v>
       </c>
       <c r="E272" t="n">
-        <v>0.0718</v>
+        <v>0.1618</v>
       </c>
     </row>
     <row r="273">
@@ -5610,13 +5610,13 @@
         </is>
       </c>
       <c r="C273" s="2" t="n">
-        <v>45532.09122685185</v>
+        <v>45532.0422800926</v>
       </c>
       <c r="D273" t="n">
-        <v>0.1287</v>
+        <v>0.114</v>
       </c>
       <c r="E273" t="n">
-        <v>0.1088</v>
+        <v>0.1375</v>
       </c>
     </row>
     <row r="274">
@@ -5629,13 +5629,13 @@
         </is>
       </c>
       <c r="C274" s="2" t="n">
-        <v>45532.09123842593</v>
+        <v>45532.04229166666</v>
       </c>
       <c r="D274" t="n">
-        <v>0.1487</v>
+        <v>0.0924</v>
       </c>
       <c r="E274" t="n">
-        <v>0.1287</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="275">
@@ -5648,13 +5648,13 @@
         </is>
       </c>
       <c r="C275" s="2" t="n">
-        <v>45532.09125</v>
+        <v>45532.04230324074</v>
       </c>
       <c r="D275" t="n">
-        <v>0.1748</v>
+        <v>0.0716</v>
       </c>
       <c r="E275" t="n">
-        <v>0.1487</v>
+        <v>0.0924</v>
       </c>
     </row>
     <row r="276">
@@ -5667,13 +5667,13 @@
         </is>
       </c>
       <c r="C276" s="2" t="n">
-        <v>45532.09126157407</v>
+        <v>45532.04236111111</v>
       </c>
       <c r="D276" t="n">
-        <v>0.2008</v>
+        <v>0.0602</v>
       </c>
       <c r="E276" t="n">
-        <v>0.1748</v>
+        <v>0.0716</v>
       </c>
     </row>
     <row r="277">
@@ -5686,13 +5686,13 @@
         </is>
       </c>
       <c r="C277" s="2" t="n">
-        <v>45532.09127314815</v>
+        <v>45532.04238425926</v>
       </c>
       <c r="D277" t="n">
-        <v>0.2185</v>
+        <v>0.06419999999999999</v>
       </c>
       <c r="E277" t="n">
-        <v>0.2008</v>
+        <v>0.0602</v>
       </c>
     </row>
     <row r="278">
@@ -5705,13 +5705,13 @@
         </is>
       </c>
       <c r="C278" s="2" t="n">
-        <v>45532.09128472222</v>
+        <v>45532.09120370371</v>
       </c>
       <c r="D278" t="n">
-        <v>0.2444</v>
+        <v>0.0718</v>
       </c>
       <c r="E278" t="n">
-        <v>0.2185</v>
+        <v>0.06419999999999999</v>
       </c>
     </row>
     <row r="279">
@@ -5724,13 +5724,13 @@
         </is>
       </c>
       <c r="C279" s="2" t="n">
-        <v>45532.0912962963</v>
+        <v>45532.09121527777</v>
       </c>
       <c r="D279" t="n">
-        <v>0.2732</v>
+        <v>0.1088</v>
       </c>
       <c r="E279" t="n">
-        <v>0.2444</v>
+        <v>0.0718</v>
       </c>
     </row>
     <row r="280">
@@ -5743,13 +5743,13 @@
         </is>
       </c>
       <c r="C280" s="2" t="n">
-        <v>45532.09130787037</v>
+        <v>45532.09122685185</v>
       </c>
       <c r="D280" t="n">
-        <v>0.2836</v>
+        <v>0.1287</v>
       </c>
       <c r="E280" t="n">
-        <v>0.2732</v>
+        <v>0.1088</v>
       </c>
     </row>
     <row r="281">
@@ -5762,13 +5762,13 @@
         </is>
       </c>
       <c r="C281" s="2" t="n">
-        <v>45532.09508101852</v>
+        <v>45532.09123842593</v>
       </c>
       <c r="D281" t="n">
-        <v>0.2701</v>
+        <v>0.1487</v>
       </c>
       <c r="E281" t="n">
-        <v>0.2836</v>
+        <v>0.1287</v>
       </c>
     </row>
     <row r="282">
@@ -5781,13 +5781,13 @@
         </is>
       </c>
       <c r="C282" s="2" t="n">
-        <v>45532.09511574074</v>
+        <v>45532.09125</v>
       </c>
       <c r="D282" t="n">
-        <v>0.232</v>
+        <v>0.1748</v>
       </c>
       <c r="E282" t="n">
-        <v>0.2701</v>
+        <v>0.1487</v>
       </c>
     </row>
     <row r="283">
@@ -5800,13 +5800,13 @@
         </is>
       </c>
       <c r="C283" s="2" t="n">
-        <v>45532.09511574074</v>
+        <v>45532.09126157407</v>
       </c>
       <c r="D283" t="n">
-        <v>0.2188</v>
+        <v>0.2008</v>
       </c>
       <c r="E283" t="n">
-        <v>0.232</v>
+        <v>0.1748</v>
       </c>
     </row>
     <row r="284">
@@ -5819,13 +5819,13 @@
         </is>
       </c>
       <c r="C284" s="2" t="n">
-        <v>45532.09512731482</v>
+        <v>45532.09127314815</v>
       </c>
       <c r="D284" t="n">
-        <v>0.1804</v>
+        <v>0.2185</v>
       </c>
       <c r="E284" t="n">
-        <v>0.2188</v>
+        <v>0.2008</v>
       </c>
     </row>
     <row r="285">
@@ -5838,13 +5838,13 @@
         </is>
       </c>
       <c r="C285" s="2" t="n">
-        <v>45532.09513888889</v>
+        <v>45532.09128472222</v>
       </c>
       <c r="D285" t="n">
-        <v>0.1608</v>
+        <v>0.2444</v>
       </c>
       <c r="E285" t="n">
-        <v>0.1804</v>
+        <v>0.2185</v>
       </c>
     </row>
     <row r="286">
@@ -5857,13 +5857,13 @@
         </is>
       </c>
       <c r="C286" s="2" t="n">
-        <v>45532.09515046296</v>
+        <v>45532.0912962963</v>
       </c>
       <c r="D286" t="n">
-        <v>0.135</v>
+        <v>0.2732</v>
       </c>
       <c r="E286" t="n">
-        <v>0.1608</v>
+        <v>0.2444</v>
       </c>
     </row>
     <row r="287">
@@ -5876,13 +5876,13 @@
         </is>
       </c>
       <c r="C287" s="2" t="n">
-        <v>45532.09516203704</v>
+        <v>45532.09130787037</v>
       </c>
       <c r="D287" t="n">
-        <v>0.1054</v>
+        <v>0.2836</v>
       </c>
       <c r="E287" t="n">
-        <v>0.135</v>
+        <v>0.2732</v>
       </c>
     </row>
     <row r="288">
@@ -5895,13 +5895,13 @@
         </is>
       </c>
       <c r="C288" s="2" t="n">
-        <v>45532.09518518519</v>
+        <v>45532.09508101852</v>
       </c>
       <c r="D288" t="n">
-        <v>0.0747</v>
+        <v>0.2701</v>
       </c>
       <c r="E288" t="n">
-        <v>0.1054</v>
+        <v>0.2836</v>
       </c>
     </row>
     <row r="289">
@@ -5914,13 +5914,13 @@
         </is>
       </c>
       <c r="C289" s="2" t="n">
-        <v>45532.09519675926</v>
+        <v>45532.09511574074</v>
       </c>
       <c r="D289" t="n">
-        <v>0.06619999999999999</v>
+        <v>0.232</v>
       </c>
       <c r="E289" t="n">
-        <v>0.0747</v>
+        <v>0.2701</v>
       </c>
     </row>
     <row r="290">
@@ -5933,13 +5933,13 @@
         </is>
       </c>
       <c r="C290" s="2" t="n">
-        <v>45532.09519675926</v>
+        <v>45532.09511574074</v>
       </c>
       <c r="D290" t="n">
-        <v>0.0638</v>
+        <v>0.2188</v>
       </c>
       <c r="E290" t="n">
-        <v>0.06619999999999999</v>
+        <v>0.232</v>
       </c>
     </row>
     <row r="291">
@@ -5952,13 +5952,13 @@
         </is>
       </c>
       <c r="C291" s="2" t="n">
-        <v>45532.19520833333</v>
+        <v>45532.09512731482</v>
       </c>
       <c r="D291" t="n">
-        <v>0.0794</v>
+        <v>0.1804</v>
       </c>
       <c r="E291" t="n">
-        <v>0.0638</v>
+        <v>0.2188</v>
       </c>
     </row>
     <row r="292">
@@ -5971,13 +5971,13 @@
         </is>
       </c>
       <c r="C292" s="2" t="n">
-        <v>45532.19521990741</v>
+        <v>45532.09513888889</v>
       </c>
       <c r="D292" t="n">
-        <v>0.1105</v>
+        <v>0.1608</v>
       </c>
       <c r="E292" t="n">
-        <v>0.0794</v>
+        <v>0.1804</v>
       </c>
     </row>
     <row r="293">
@@ -5990,13 +5990,13 @@
         </is>
       </c>
       <c r="C293" s="2" t="n">
-        <v>45532.19523148148</v>
+        <v>45532.09515046296</v>
       </c>
       <c r="D293" t="n">
-        <v>0.1384</v>
+        <v>0.135</v>
       </c>
       <c r="E293" t="n">
-        <v>0.1105</v>
+        <v>0.1608</v>
       </c>
     </row>
     <row r="294">
@@ -6009,13 +6009,13 @@
         </is>
       </c>
       <c r="C294" s="2" t="n">
-        <v>45532.19524305555</v>
+        <v>45532.09516203704</v>
       </c>
       <c r="D294" t="n">
-        <v>0.1596</v>
+        <v>0.1054</v>
       </c>
       <c r="E294" t="n">
-        <v>0.1384</v>
+        <v>0.135</v>
       </c>
     </row>
     <row r="295">
@@ -6028,13 +6028,13 @@
         </is>
       </c>
       <c r="C295" s="2" t="n">
-        <v>45532.19525462963</v>
+        <v>45532.09518518519</v>
       </c>
       <c r="D295" t="n">
-        <v>0.1807</v>
+        <v>0.0747</v>
       </c>
       <c r="E295" t="n">
-        <v>0.1596</v>
+        <v>0.1054</v>
       </c>
     </row>
     <row r="296">
@@ -6047,13 +6047,13 @@
         </is>
       </c>
       <c r="C296" s="2" t="n">
-        <v>45532.1952662037</v>
+        <v>45532.09519675926</v>
       </c>
       <c r="D296" t="n">
-        <v>0.2032</v>
+        <v>0.06619999999999999</v>
       </c>
       <c r="E296" t="n">
-        <v>0.1807</v>
+        <v>0.0747</v>
       </c>
     </row>
     <row r="297">
@@ -6066,13 +6066,13 @@
         </is>
       </c>
       <c r="C297" s="2" t="n">
-        <v>45532.19527777778</v>
+        <v>45532.09519675926</v>
       </c>
       <c r="D297" t="n">
-        <v>0.2208</v>
+        <v>0.0638</v>
       </c>
       <c r="E297" t="n">
-        <v>0.2032</v>
+        <v>0.06619999999999999</v>
       </c>
     </row>
     <row r="298">
@@ -6085,13 +6085,13 @@
         </is>
       </c>
       <c r="C298" s="2" t="n">
-        <v>45532.19825231482</v>
+        <v>45532.19520833333</v>
       </c>
       <c r="D298" t="n">
-        <v>0.2073</v>
+        <v>0.0794</v>
       </c>
       <c r="E298" t="n">
-        <v>0.2208</v>
+        <v>0.0638</v>
       </c>
     </row>
     <row r="299">
@@ -6104,13 +6104,13 @@
         </is>
       </c>
       <c r="C299" s="2" t="n">
-        <v>45532.19826388889</v>
+        <v>45532.19521990741</v>
       </c>
       <c r="D299" t="n">
-        <v>0.1902</v>
+        <v>0.1105</v>
       </c>
       <c r="E299" t="n">
-        <v>0.2073</v>
+        <v>0.0794</v>
       </c>
     </row>
     <row r="300">
@@ -6123,13 +6123,13 @@
         </is>
       </c>
       <c r="C300" s="2" t="n">
-        <v>45532.19827546296</v>
+        <v>45532.19523148148</v>
       </c>
       <c r="D300" t="n">
-        <v>0.1629</v>
+        <v>0.1384</v>
       </c>
       <c r="E300" t="n">
-        <v>0.1902</v>
+        <v>0.1105</v>
       </c>
     </row>
     <row r="301">
@@ -6142,13 +6142,13 @@
         </is>
       </c>
       <c r="C301" s="2" t="n">
-        <v>45532.19828703703</v>
+        <v>45532.19524305555</v>
       </c>
       <c r="D301" t="n">
-        <v>0.1392</v>
+        <v>0.1596</v>
       </c>
       <c r="E301" t="n">
-        <v>0.1629</v>
+        <v>0.1384</v>
       </c>
     </row>
     <row r="302">
@@ -6161,13 +6161,13 @@
         </is>
       </c>
       <c r="C302" s="2" t="n">
-        <v>45532.19829861111</v>
+        <v>45532.19525462963</v>
       </c>
       <c r="D302" t="n">
-        <v>0.1117</v>
+        <v>0.1807</v>
       </c>
       <c r="E302" t="n">
-        <v>0.1392</v>
+        <v>0.1596</v>
       </c>
     </row>
     <row r="303">
@@ -6180,13 +6180,13 @@
         </is>
       </c>
       <c r="C303" s="2" t="n">
-        <v>45532.19831018519</v>
+        <v>45532.1952662037</v>
       </c>
       <c r="D303" t="n">
-        <v>0.091</v>
+        <v>0.2032</v>
       </c>
       <c r="E303" t="n">
-        <v>0.1117</v>
+        <v>0.1807</v>
       </c>
     </row>
     <row r="304">
@@ -6199,13 +6199,13 @@
         </is>
       </c>
       <c r="C304" s="2" t="n">
-        <v>45532.19832175926</v>
+        <v>45532.19527777778</v>
       </c>
       <c r="D304" t="n">
-        <v>0.076</v>
+        <v>0.2208</v>
       </c>
       <c r="E304" t="n">
-        <v>0.091</v>
+        <v>0.2032</v>
       </c>
     </row>
     <row r="305">
@@ -6218,13 +6218,13 @@
         </is>
       </c>
       <c r="C305" s="2" t="n">
-        <v>45532.19833333333</v>
+        <v>45532.19825231482</v>
       </c>
       <c r="D305" t="n">
-        <v>0.06270000000000001</v>
+        <v>0.2073</v>
       </c>
       <c r="E305" t="n">
-        <v>0.076</v>
+        <v>0.2208</v>
       </c>
     </row>
     <row r="306">
@@ -6237,13 +6237,13 @@
         </is>
       </c>
       <c r="C306" s="2" t="n">
-        <v>45532.19834490741</v>
+        <v>45532.19826388889</v>
       </c>
       <c r="D306" t="n">
-        <v>0.055</v>
+        <v>0.1902</v>
       </c>
       <c r="E306" t="n">
-        <v>0.06270000000000001</v>
+        <v>0.2073</v>
       </c>
     </row>
     <row r="307">
@@ -6256,13 +6256,13 @@
         </is>
       </c>
       <c r="C307" s="2" t="n">
-        <v>45532.19836805556</v>
+        <v>45532.19827546296</v>
       </c>
       <c r="D307" t="n">
-        <v>0.056</v>
+        <v>0.1629</v>
       </c>
       <c r="E307" t="n">
-        <v>0.055</v>
+        <v>0.1902</v>
       </c>
     </row>
     <row r="308">
@@ -6275,13 +6275,13 @@
         </is>
       </c>
       <c r="C308" s="2" t="n">
-        <v>45532.19837962963</v>
+        <v>45532.19828703703</v>
       </c>
       <c r="D308" t="n">
-        <v>0.0589</v>
+        <v>0.1392</v>
       </c>
       <c r="E308" t="n">
-        <v>0.056</v>
+        <v>0.1629</v>
       </c>
     </row>
     <row r="309">
@@ -6294,13 +6294,13 @@
         </is>
       </c>
       <c r="C309" s="2" t="n">
-        <v>45532.1983912037</v>
+        <v>45532.19829861111</v>
       </c>
       <c r="D309" t="n">
-        <v>0.062</v>
+        <v>0.1117</v>
       </c>
       <c r="E309" t="n">
-        <v>0.0589</v>
+        <v>0.1392</v>
       </c>
     </row>
     <row r="310">
@@ -6313,13 +6313,13 @@
         </is>
       </c>
       <c r="C310" s="2" t="n">
-        <v>45532.19840277778</v>
+        <v>45532.19831018519</v>
       </c>
       <c r="D310" t="n">
-        <v>0.0635</v>
+        <v>0.091</v>
       </c>
       <c r="E310" t="n">
-        <v>0.062</v>
+        <v>0.1117</v>
       </c>
     </row>
     <row r="311">
@@ -6332,13 +6332,13 @@
         </is>
       </c>
       <c r="C311" s="2" t="n">
-        <v>45532.22447916667</v>
+        <v>45532.19832175926</v>
       </c>
       <c r="D311" t="n">
-        <v>0.06279999999999999</v>
+        <v>0.076</v>
       </c>
       <c r="E311" t="n">
-        <v>0.0635</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="312">
@@ -6351,13 +6351,13 @@
         </is>
       </c>
       <c r="C312" s="2" t="n">
-        <v>45532.30078703703</v>
+        <v>45532.19833333333</v>
       </c>
       <c r="D312" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.06270000000000001</v>
       </c>
       <c r="E312" t="n">
-        <v>0.06279999999999999</v>
+        <v>0.076</v>
       </c>
     </row>
     <row r="313">
@@ -6370,13 +6370,13 @@
         </is>
       </c>
       <c r="C313" s="2" t="n">
-        <v>45532.30081018519</v>
+        <v>45532.19834490741</v>
       </c>
       <c r="D313" t="n">
-        <v>0.1157</v>
+        <v>0.055</v>
       </c>
       <c r="E313" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.06270000000000001</v>
       </c>
     </row>
     <row r="314">
@@ -6389,13 +6389,13 @@
         </is>
       </c>
       <c r="C314" s="2" t="n">
-        <v>45532.30081018519</v>
+        <v>45532.19836805556</v>
       </c>
       <c r="D314" t="n">
-        <v>0.1329</v>
+        <v>0.056</v>
       </c>
       <c r="E314" t="n">
-        <v>0.1157</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="315">
@@ -6408,13 +6408,13 @@
         </is>
       </c>
       <c r="C315" s="2" t="n">
-        <v>45532.30082175926</v>
+        <v>45532.19837962963</v>
       </c>
       <c r="D315" t="n">
-        <v>0.1525</v>
+        <v>0.0589</v>
       </c>
       <c r="E315" t="n">
-        <v>0.1329</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="316">
@@ -6427,13 +6427,13 @@
         </is>
       </c>
       <c r="C316" s="2" t="n">
-        <v>45532.30083333333</v>
+        <v>45532.1983912037</v>
       </c>
       <c r="D316" t="n">
-        <v>0.1844</v>
+        <v>0.062</v>
       </c>
       <c r="E316" t="n">
-        <v>0.1525</v>
+        <v>0.0589</v>
       </c>
     </row>
     <row r="317">
@@ -6446,13 +6446,13 @@
         </is>
       </c>
       <c r="C317" s="2" t="n">
-        <v>45532.3008449074</v>
+        <v>45532.19840277778</v>
       </c>
       <c r="D317" t="n">
-        <v>0.1966</v>
+        <v>0.0635</v>
       </c>
       <c r="E317" t="n">
-        <v>0.1844</v>
+        <v>0.062</v>
       </c>
     </row>
     <row r="318">
@@ -6465,13 +6465,13 @@
         </is>
       </c>
       <c r="C318" s="2" t="n">
-        <v>45532.30197916667</v>
+        <v>45532.22447916667</v>
       </c>
       <c r="D318" t="n">
-        <v>0.1806</v>
+        <v>0.06279999999999999</v>
       </c>
       <c r="E318" t="n">
-        <v>0.1966</v>
+        <v>0.0635</v>
       </c>
     </row>
     <row r="319">
@@ -6484,13 +6484,13 @@
         </is>
       </c>
       <c r="C319" s="2" t="n">
-        <v>45532.30199074074</v>
+        <v>45532.30078703703</v>
       </c>
       <c r="D319" t="n">
-        <v>0.1452</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="E319" t="n">
-        <v>0.1806</v>
+        <v>0.06279999999999999</v>
       </c>
     </row>
     <row r="320">
@@ -6503,13 +6503,13 @@
         </is>
       </c>
       <c r="C320" s="2" t="n">
-        <v>45532.30200231481</v>
+        <v>45532.30081018519</v>
       </c>
       <c r="D320" t="n">
-        <v>0.1252</v>
+        <v>0.1157</v>
       </c>
       <c r="E320" t="n">
-        <v>0.1452</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="321">
@@ -6522,13 +6522,13 @@
         </is>
       </c>
       <c r="C321" s="2" t="n">
-        <v>45532.30201388889</v>
+        <v>45532.30081018519</v>
       </c>
       <c r="D321" t="n">
-        <v>0.1067</v>
+        <v>0.1329</v>
       </c>
       <c r="E321" t="n">
-        <v>0.1252</v>
+        <v>0.1157</v>
       </c>
     </row>
     <row r="322">
@@ -6541,13 +6541,13 @@
         </is>
       </c>
       <c r="C322" s="2" t="n">
-        <v>45532.30202546297</v>
+        <v>45532.30082175926</v>
       </c>
       <c r="D322" t="n">
-        <v>0.08210000000000001</v>
+        <v>0.1525</v>
       </c>
       <c r="E322" t="n">
-        <v>0.1067</v>
+        <v>0.1329</v>
       </c>
     </row>
     <row r="323">
@@ -6560,13 +6560,13 @@
         </is>
       </c>
       <c r="C323" s="2" t="n">
-        <v>45532.30203703704</v>
+        <v>45532.30083333333</v>
       </c>
       <c r="D323" t="n">
-        <v>0.0697</v>
+        <v>0.1844</v>
       </c>
       <c r="E323" t="n">
-        <v>0.08210000000000001</v>
+        <v>0.1525</v>
       </c>
     </row>
     <row r="324">
@@ -6579,13 +6579,13 @@
         </is>
       </c>
       <c r="C324" s="2" t="n">
-        <v>45532.30204861111</v>
+        <v>45532.3008449074</v>
       </c>
       <c r="D324" t="n">
-        <v>0.0612</v>
+        <v>0.1966</v>
       </c>
       <c r="E324" t="n">
-        <v>0.0697</v>
+        <v>0.1844</v>
       </c>
     </row>
     <row r="325">
@@ -6598,13 +6598,13 @@
         </is>
       </c>
       <c r="C325" s="2" t="n">
-        <v>45532.30206018518</v>
+        <v>45532.30197916667</v>
       </c>
       <c r="D325" t="n">
-        <v>0.054</v>
+        <v>0.1806</v>
       </c>
       <c r="E325" t="n">
-        <v>0.0612</v>
+        <v>0.1966</v>
       </c>
     </row>
     <row r="326">
@@ -6617,13 +6617,13 @@
         </is>
       </c>
       <c r="C326" s="2" t="n">
-        <v>45532.30207175926</v>
+        <v>45532.30199074074</v>
       </c>
       <c r="D326" t="n">
-        <v>0.0547</v>
+        <v>0.1452</v>
       </c>
       <c r="E326" t="n">
-        <v>0.054</v>
+        <v>0.1806</v>
       </c>
     </row>
     <row r="327">
@@ -6636,13 +6636,13 @@
         </is>
       </c>
       <c r="C327" s="2" t="n">
-        <v>45532.30208333334</v>
+        <v>45532.30200231481</v>
       </c>
       <c r="D327" t="n">
-        <v>0.0623</v>
+        <v>0.1252</v>
       </c>
       <c r="E327" t="n">
-        <v>0.0547</v>
+        <v>0.1452</v>
       </c>
     </row>
     <row r="328">
@@ -6655,13 +6655,13 @@
         </is>
       </c>
       <c r="C328" s="2" t="n">
-        <v>45532.30210648148</v>
+        <v>45532.30201388889</v>
       </c>
       <c r="D328" t="n">
-        <v>0.0634</v>
+        <v>0.1067</v>
       </c>
       <c r="E328" t="n">
-        <v>0.0623</v>
+        <v>0.1252</v>
       </c>
     </row>
     <row r="329">
@@ -6674,13 +6674,13 @@
         </is>
       </c>
       <c r="C329" s="2" t="n">
-        <v>45532.30210648148</v>
+        <v>45532.30202546297</v>
       </c>
       <c r="D329" t="n">
-        <v>0.0625</v>
+        <v>0.08210000000000001</v>
       </c>
       <c r="E329" t="n">
-        <v>0.0634</v>
+        <v>0.1067</v>
       </c>
     </row>
     <row r="330">
@@ -6689,16 +6689,18 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C330" s="2" t="n">
-        <v>45531.875</v>
+        <v>45532.30203703704</v>
       </c>
       <c r="D330" t="n">
-        <v>65</v>
-      </c>
-      <c r="E330" t="inlineStr"/>
+        <v>0.0697</v>
+      </c>
+      <c r="E330" t="n">
+        <v>0.08210000000000001</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -6706,17 +6708,17 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C331" s="2" t="n">
-        <v>45532.00697916667</v>
+        <v>45532.30204861111</v>
       </c>
       <c r="D331" t="n">
-        <v>60</v>
+        <v>0.0612</v>
       </c>
       <c r="E331" t="n">
-        <v>65</v>
+        <v>0.0697</v>
       </c>
     </row>
     <row r="332">
@@ -6725,17 +6727,17 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C332" s="2" t="n">
-        <v>45532.01064814815</v>
+        <v>45532.30206018518</v>
       </c>
       <c r="D332" t="n">
-        <v>65</v>
+        <v>0.054</v>
       </c>
       <c r="E332" t="n">
-        <v>60</v>
+        <v>0.0612</v>
       </c>
     </row>
     <row r="333">
@@ -6744,17 +6746,17 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C333" s="2" t="n">
-        <v>45532.01260416667</v>
+        <v>45532.30207175926</v>
       </c>
       <c r="D333" t="n">
-        <v>63</v>
+        <v>0.0547</v>
       </c>
       <c r="E333" t="n">
-        <v>65</v>
+        <v>0.054</v>
       </c>
     </row>
     <row r="334">
@@ -6763,17 +6765,17 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C334" s="2" t="n">
-        <v>45532.05307870371</v>
+        <v>45532.30208333334</v>
       </c>
       <c r="D334" t="n">
-        <v>65</v>
+        <v>0.0623</v>
       </c>
       <c r="E334" t="n">
-        <v>63</v>
+        <v>0.0547</v>
       </c>
     </row>
     <row r="335">
@@ -6782,17 +6784,17 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C335" s="2" t="n">
-        <v>45532.06596064815</v>
+        <v>45532.30210648148</v>
       </c>
       <c r="D335" t="n">
-        <v>60</v>
+        <v>0.0634</v>
       </c>
       <c r="E335" t="n">
-        <v>65</v>
+        <v>0.0623</v>
       </c>
     </row>
     <row r="336">
@@ -6801,17 +6803,17 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+          <t>CG_Sheeting.CG_Sheeting.dbHMI.Sheeting.SRV_GapFinalSizing.rActualPosition_inches</t>
         </is>
       </c>
       <c r="C336" s="2" t="n">
-        <v>45532.1430787037</v>
+        <v>45532.30210648148</v>
       </c>
       <c r="D336" t="n">
-        <v>65</v>
+        <v>0.0625</v>
       </c>
       <c r="E336" t="n">
-        <v>60</v>
+        <v>0.0634</v>
       </c>
     </row>
     <row r="337">
@@ -6824,14 +6826,12 @@
         </is>
       </c>
       <c r="C337" s="2" t="n">
-        <v>45532.14484953704</v>
+        <v>45531.875</v>
       </c>
       <c r="D337" t="n">
-        <v>60</v>
-      </c>
-      <c r="E337" t="n">
         <v>65</v>
       </c>
+      <c r="E337" t="inlineStr"/>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
@@ -6843,13 +6843,13 @@
         </is>
       </c>
       <c r="C338" s="2" t="n">
-        <v>45532.17368055556</v>
+        <v>45532.00697916667</v>
       </c>
       <c r="D338" t="n">
+        <v>60</v>
+      </c>
+      <c r="E338" t="n">
         <v>65</v>
-      </c>
-      <c r="E338" t="n">
-        <v>60</v>
       </c>
     </row>
     <row r="339">
@@ -6862,12 +6862,145 @@
         </is>
       </c>
       <c r="C339" s="2" t="n">
+        <v>45532.01064814815</v>
+      </c>
+      <c r="D339" t="n">
+        <v>65</v>
+      </c>
+      <c r="E339" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1" t="n">
+        <v>338</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+        </is>
+      </c>
+      <c r="C340" s="2" t="n">
+        <v>45532.01260416667</v>
+      </c>
+      <c r="D340" t="n">
+        <v>63</v>
+      </c>
+      <c r="E340" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1" t="n">
+        <v>339</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+        </is>
+      </c>
+      <c r="C341" s="2" t="n">
+        <v>45532.05307870371</v>
+      </c>
+      <c r="D341" t="n">
+        <v>65</v>
+      </c>
+      <c r="E341" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+        </is>
+      </c>
+      <c r="C342" s="2" t="n">
+        <v>45532.06596064815</v>
+      </c>
+      <c r="D342" t="n">
+        <v>60</v>
+      </c>
+      <c r="E342" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1" t="n">
+        <v>341</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+        </is>
+      </c>
+      <c r="C343" s="2" t="n">
+        <v>45532.1430787037</v>
+      </c>
+      <c r="D343" t="n">
+        <v>65</v>
+      </c>
+      <c r="E343" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+        </is>
+      </c>
+      <c r="C344" s="2" t="n">
+        <v>45532.14484953704</v>
+      </c>
+      <c r="D344" t="n">
+        <v>60</v>
+      </c>
+      <c r="E344" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+        </is>
+      </c>
+      <c r="C345" s="2" t="n">
+        <v>45532.17368055556</v>
+      </c>
+      <c r="D345" t="n">
+        <v>65</v>
+      </c>
+      <c r="E345" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>SFBMix.PLC_BOSCH EXTRUDER.DB_Data_Exchange.EXT_PH_Temp_SP</t>
+        </is>
+      </c>
+      <c r="C346" s="2" t="n">
         <v>45532.17561342593</v>
       </c>
-      <c r="D339" t="n">
+      <c r="D346" t="n">
         <v>30</v>
       </c>
-      <c r="E339" t="n">
+      <c r="E346" t="n">
         <v>65</v>
       </c>
     </row>

</xml_diff>